<commit_message>
pushing protocols to the repo. July 2018
</commit_message>
<xml_diff>
--- a/solutions/dilutions_calculations.xlsx
+++ b/solutions/dilutions_calculations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,11 +63,11 @@
     <definedName name="solver_typ" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">1000</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0.7</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0.8</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -110,8 +110,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,12 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -175,6 +183,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -223,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,9 +267,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,6 +319,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,11 +511,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,14 +539,14 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>0.4285720154146348</v>
+        <v>3.7499897640840105</v>
       </c>
       <c r="D2">
         <f>B2*A2/SUM(B2:C2)</f>
-        <v>0.69999971244694703</v>
+        <v>0.80000043673265397</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -509,21 +554,19 @@
         <v>0.95</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>0.35714311715140845</v>
+        <v>1.8750063944342681</v>
       </c>
       <c r="D3">
         <f>B3*A3/SUM(B3:C3)</f>
-        <v>0.6999998658903519</v>
+        <v>0.79999956921729187</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3">
-        <v>0.7</v>
-      </c>
+      <c r="G3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -531,59 +574,60 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <f>(B2-1)*B6</f>
         <v>980</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <f>SUM(B6:B8)</f>
         <v>1000</v>
       </c>
@@ -594,7 +638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>